<commit_message>
Sincronizar manual computadora shadi de deposito (hafiz probablemente)
</commit_message>
<xml_diff>
--- a/INVENTARIOS DEPOSITO/11-07-2022/11-7-2022 HAFIZ MESTRE.xlsx
+++ b/INVENTARIOS DEPOSITO/11-07-2022/11-7-2022 HAFIZ MESTRE.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABDALLA\Desktop\INVENTARIOS\INVENTARIOS TIENDA\11-07-2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chadi Salloum\Desktop\INVENTARIOS\INVENTARIOS DEPOSITO\11-07-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC33074-CF9E-4508-B92B-744D32C9416E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78295ABE-F1D1-4491-8E3A-EA4EEF4F19FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="68">
   <si>
     <t>CO_ART</t>
   </si>
@@ -138,66 +138,36 @@
     <t>CVB35BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI12</t>
-  </si>
-  <si>
     <t>CVB36BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI13</t>
-  </si>
-  <si>
     <t>CVB37BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI14</t>
-  </si>
-  <si>
     <t>CVB38BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI15</t>
-  </si>
-  <si>
     <t>CVB39BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI16</t>
-  </si>
-  <si>
     <t>CVB40BT-30003</t>
   </si>
   <si>
     <t>CABALLERO</t>
   </si>
   <si>
-    <t>0005700003577CI17</t>
-  </si>
-  <si>
     <t>CVB41BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI18</t>
-  </si>
-  <si>
     <t>CVB42BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI19</t>
-  </si>
-  <si>
     <t>CVB43BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI20</t>
-  </si>
-  <si>
     <t>CVB44BT-30003</t>
   </si>
   <si>
-    <t>0005700003577CI21</t>
-  </si>
-  <si>
     <t>CVN34BT-20002</t>
   </si>
   <si>
@@ -207,69 +177,36 @@
     <t>NEGRO</t>
   </si>
   <si>
-    <t>0005700003577CI22</t>
-  </si>
-  <si>
     <t>CVN35BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI23</t>
-  </si>
-  <si>
     <t>CVN36BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI24</t>
-  </si>
-  <si>
     <t>CVN37BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI25</t>
-  </si>
-  <si>
     <t>CVN38BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI26</t>
-  </si>
-  <si>
     <t>CVN39BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI27</t>
-  </si>
-  <si>
     <t>CVN40BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI28</t>
-  </si>
-  <si>
     <t>CVN41BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI29</t>
-  </si>
-  <si>
     <t>CVN42BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI30</t>
-  </si>
-  <si>
     <t>CVN43BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI31</t>
-  </si>
-  <si>
     <t>CVN44BT-20002</t>
   </si>
   <si>
-    <t>0005700003577CI32</t>
-  </si>
-  <si>
     <t>CVA34BT-10001</t>
   </si>
   <si>
@@ -289,24 +226,6 @@
   </si>
   <si>
     <t>AZUL</t>
-  </si>
-  <si>
-    <t>0005700003577CI33</t>
-  </si>
-  <si>
-    <t>0005700003577CI34</t>
-  </si>
-  <si>
-    <t>0005700003577CI35</t>
-  </si>
-  <si>
-    <t>0005700003577CI36</t>
-  </si>
-  <si>
-    <t>0005700003577CI37</t>
-  </si>
-  <si>
-    <t>0005700003577CI38</t>
   </si>
   <si>
     <t>CVA43BT-10001</t>
@@ -474,7 +393,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -770,13 +689,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="C36:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
@@ -915,9 +834,6 @@
       <c r="V2" t="s">
         <v>34</v>
       </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
       <c r="X2">
         <v>25998807</v>
       </c>
@@ -972,10 +888,7 @@
         <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X3">
         <v>25998807</v>
@@ -989,7 +902,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -1031,10 +944,7 @@
         <v>15</v>
       </c>
       <c r="V4" t="s">
-        <v>39</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X4">
         <v>25998807</v>
@@ -1048,7 +958,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -1090,10 +1000,7 @@
         <v>15</v>
       </c>
       <c r="V5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X5">
         <v>25998807</v>
@@ -1107,7 +1014,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -1149,10 +1056,7 @@
         <v>15</v>
       </c>
       <c r="V6" t="s">
-        <v>43</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X6">
         <v>25998807</v>
@@ -1166,7 +1070,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -1208,10 +1112,7 @@
         <v>15</v>
       </c>
       <c r="V7" t="s">
-        <v>45</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X7">
         <v>25998807</v>
@@ -1225,7 +1126,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
@@ -1234,7 +1135,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -1267,10 +1168,7 @@
         <v>15</v>
       </c>
       <c r="V8" t="s">
-        <v>48</v>
-      </c>
-      <c r="W8">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X8">
         <v>25998807</v>
@@ -1284,7 +1182,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1293,7 +1191,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1326,10 +1224,7 @@
         <v>15</v>
       </c>
       <c r="V9" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X9">
         <v>25998807</v>
@@ -1343,7 +1238,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1352,7 +1247,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -1385,10 +1280,7 @@
         <v>15</v>
       </c>
       <c r="V10" t="s">
-        <v>52</v>
-      </c>
-      <c r="W10">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X10">
         <v>25998807</v>
@@ -1402,7 +1294,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -1411,7 +1303,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -1444,10 +1336,7 @@
         <v>15</v>
       </c>
       <c r="V11" t="s">
-        <v>54</v>
-      </c>
-      <c r="W11">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X11">
         <v>25998807</v>
@@ -1461,7 +1350,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1470,7 +1359,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -1503,10 +1392,7 @@
         <v>15</v>
       </c>
       <c r="V12" t="s">
-        <v>56</v>
-      </c>
-      <c r="W12">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X12">
         <v>25998807</v>
@@ -1520,10 +1406,10 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
@@ -1544,7 +1430,7 @@
         <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J13">
         <v>34</v>
@@ -1562,10 +1448,7 @@
         <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>60</v>
-      </c>
-      <c r="W13">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X13">
         <v>25998807</v>
@@ -1579,10 +1462,10 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
@@ -1603,7 +1486,7 @@
         <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J14">
         <v>35</v>
@@ -1621,10 +1504,7 @@
         <v>15</v>
       </c>
       <c r="V14" t="s">
-        <v>62</v>
-      </c>
-      <c r="W14">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X14">
         <v>25998807</v>
@@ -1638,10 +1518,10 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -1662,7 +1542,7 @@
         <v>32</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J15">
         <v>36</v>
@@ -1680,10 +1560,7 @@
         <v>15</v>
       </c>
       <c r="V15" t="s">
-        <v>64</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X15">
         <v>25998807</v>
@@ -1697,10 +1574,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1721,7 +1598,7 @@
         <v>32</v>
       </c>
       <c r="I16" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J16">
         <v>37</v>
@@ -1739,10 +1616,7 @@
         <v>15</v>
       </c>
       <c r="V16" t="s">
-        <v>66</v>
-      </c>
-      <c r="W16">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X16">
         <v>25998807</v>
@@ -1756,10 +1630,10 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
@@ -1780,7 +1654,7 @@
         <v>32</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J17">
         <v>38</v>
@@ -1798,10 +1672,7 @@
         <v>15</v>
       </c>
       <c r="V17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W17">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X17">
         <v>25998807</v>
@@ -1815,10 +1686,10 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
@@ -1839,7 +1710,7 @@
         <v>32</v>
       </c>
       <c r="I18" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J18">
         <v>39</v>
@@ -1857,10 +1728,7 @@
         <v>15</v>
       </c>
       <c r="V18" t="s">
-        <v>70</v>
-      </c>
-      <c r="W18">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X18">
         <v>25998807</v>
@@ -1874,16 +1742,16 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1898,7 +1766,7 @@
         <v>32</v>
       </c>
       <c r="I19" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J19">
         <v>40</v>
@@ -1916,10 +1784,7 @@
         <v>15</v>
       </c>
       <c r="V19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W19">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X19">
         <v>25998807</v>
@@ -1933,16 +1798,16 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -1957,7 +1822,7 @@
         <v>32</v>
       </c>
       <c r="I20" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J20">
         <v>41</v>
@@ -1975,10 +1840,7 @@
         <v>15</v>
       </c>
       <c r="V20" t="s">
-        <v>74</v>
-      </c>
-      <c r="W20">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X20">
         <v>25998807</v>
@@ -1992,16 +1854,16 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -2016,7 +1878,7 @@
         <v>32</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J21">
         <v>42</v>
@@ -2034,10 +1896,7 @@
         <v>15</v>
       </c>
       <c r="V21" t="s">
-        <v>76</v>
-      </c>
-      <c r="W21">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X21">
         <v>25998807</v>
@@ -2051,16 +1910,16 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -2075,7 +1934,7 @@
         <v>32</v>
       </c>
       <c r="I22" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J22">
         <v>43</v>
@@ -2093,10 +1952,7 @@
         <v>15</v>
       </c>
       <c r="V22" t="s">
-        <v>78</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X22">
         <v>25998807</v>
@@ -2110,16 +1966,16 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -2134,7 +1990,7 @@
         <v>32</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J23">
         <v>44</v>
@@ -2152,10 +2008,7 @@
         <v>15</v>
       </c>
       <c r="V23" t="s">
-        <v>80</v>
-      </c>
-      <c r="W23">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X23">
         <v>25998807</v>
@@ -2169,10 +2022,10 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
@@ -2193,7 +2046,7 @@
         <v>32</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J24">
         <v>34</v>
@@ -2211,10 +2064,7 @@
         <v>15</v>
       </c>
       <c r="V24" t="s">
-        <v>88</v>
-      </c>
-      <c r="W24">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X24">
         <v>25998807</v>
@@ -2228,10 +2078,10 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
@@ -2252,7 +2102,7 @@
         <v>32</v>
       </c>
       <c r="I25" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J25">
         <v>35</v>
@@ -2270,10 +2120,7 @@
         <v>15</v>
       </c>
       <c r="V25" t="s">
-        <v>89</v>
-      </c>
-      <c r="W25">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X25">
         <v>25998807</v>
@@ -2287,10 +2134,10 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -2311,7 +2158,7 @@
         <v>32</v>
       </c>
       <c r="I26" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J26">
         <v>38</v>
@@ -2329,10 +2176,7 @@
         <v>15</v>
       </c>
       <c r="V26" t="s">
-        <v>90</v>
-      </c>
-      <c r="W26">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X26">
         <v>25998807</v>
@@ -2346,10 +2190,10 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -2370,7 +2214,7 @@
         <v>32</v>
       </c>
       <c r="I27" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J27">
         <v>39</v>
@@ -2388,10 +2232,7 @@
         <v>15</v>
       </c>
       <c r="V27" t="s">
-        <v>91</v>
-      </c>
-      <c r="W27">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X27">
         <v>25998807</v>
@@ -2405,16 +2246,16 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
@@ -2429,7 +2270,7 @@
         <v>32</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J28">
         <v>43</v>
@@ -2447,10 +2288,7 @@
         <v>15</v>
       </c>
       <c r="V28" t="s">
-        <v>92</v>
-      </c>
-      <c r="W28">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X28">
         <v>25998807</v>
@@ -2464,16 +2302,16 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -2488,7 +2326,7 @@
         <v>32</v>
       </c>
       <c r="I29" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="J29">
         <v>44</v>
@@ -2506,10 +2344,7 @@
         <v>15</v>
       </c>
       <c r="V29" t="s">
-        <v>93</v>
-      </c>
-      <c r="W29">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X29">
         <v>25998807</v>
@@ -2521,6 +2356,7 @@
         <v>35</v>
       </c>
     </row>
+    <row r="36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>